<commit_message>
creadas rutinas disparo_camara, disparo_flaix, inicializacion...
</commit_message>
<xml_diff>
--- a/PinOut.xlsx
+++ b/PinOut.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$B$2:$J$31</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -859,10 +862,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1509,8 +1515,12 @@
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:J2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="1.3385826771653544" bottom="0.74803149606299213" header="0.59055118110236227" footer="0"/>
+  <pageSetup paperSize="9" scale="99" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CPINOUT PSoCs</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>